<commit_message>
some simplification in kernel5.cu
</commit_message>
<xml_diff>
--- a/variable-mapping.xlsx
+++ b/variable-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skim/Dropbox (PVAMU)/workspace-EDDY/eddy-gpu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25BBAD7E-E460-CF44-BD47-2EE270720ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C23C7D8-6C61-404C-B8CC-D3DFA2D391CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{E2CA769E-306F-9D4A-8C38-056F3DE2E5AA}"/>
   </bookViews>
@@ -202,18 +202,6 @@
     <t>(spacr, ff) gives gene pair</t>
   </si>
   <si>
-    <t>row_id</t>
-  </si>
-  <si>
-    <t>col_id</t>
-  </si>
-  <si>
-    <t>col_id of edge stored in diagonal represenation</t>
-  </si>
-  <si>
-    <t>row_id of edge stored in diagonal representation</t>
-  </si>
-  <si>
     <t>degree of freedom in chisq test</t>
   </si>
   <si>
@@ -281,6 +269,18 @@
   </si>
   <si>
     <t>length = 3 * 2 * # of genes in a geneset</t>
+  </si>
+  <si>
+    <t>row_id / gene_i</t>
+  </si>
+  <si>
+    <t>col_id / gene_j</t>
+  </si>
+  <si>
+    <t>row_id of edge stored in diagonal representation (gene_i)</t>
+  </si>
+  <si>
+    <t>col_id of edge stored in diagonal represenation (gene_j)</t>
   </si>
 </sst>
 </file>
@@ -635,14 +635,14 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29:H31"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -676,7 +676,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -715,7 +715,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
@@ -732,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -749,7 +749,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
         <v>51</v>
@@ -763,7 +763,7 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
         <v>51</v>
@@ -785,13 +785,13 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -802,13 +802,13 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -877,27 +877,27 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -905,10 +905,10 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" t="s">
         <v>61</v>
-      </c>
-      <c r="F24" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -952,13 +952,13 @@
         <v>33</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="G29" t="s">
         <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -969,7 +969,7 @@
         <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="G30" t="s">
         <v>53</v>
@@ -986,10 +986,10 @@
         <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1000,7 +1000,7 @@
         <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>